<commit_message>
Update fsl_spark from fsl_addons classes
</commit_message>
<xml_diff>
--- a/fsl-spark/src/test/results/xls/applyFontStylesItalicToRange.xlsx
+++ b/fsl-spark/src/test/results/xls/applyFontStylesItalicToRange.xlsx
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,27 +93,6 @@
       <sz val="12.0"/>
       <b val="true"/>
       <u val="none"/>
-      <color indexed="0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <i val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <u val="double"/>
       <color indexed="0"/>
     </font>
   </fonts>
@@ -202,18 +181,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
     </xf>
   </cellXfs>
@@ -551,44 +521,44 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s" s="2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" s="3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s" s="4">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplified code and added executables and support files
</commit_message>
<xml_diff>
--- a/fsl-spark/src/test/results/xls/applyFontStylesItalicToRange.xlsx
+++ b/fsl-spark/src/test/results/xls/applyFontStylesItalicToRange.xlsx
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,6 +93,27 @@
       <sz val="12.0"/>
       <b val="true"/>
       <u val="none"/>
+      <color indexed="0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+      <i val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <u val="double"/>
       <color indexed="0"/>
     </font>
   </fonts>
@@ -181,9 +202,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyAlignment="true" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" shrinkToFit="false" wrapText="false"/>
     </xf>
   </cellXfs>
@@ -521,44 +551,44 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="4">
         <v>12</v>
       </c>
     </row>

</xml_diff>